<commit_message>
Rework the organization of the .bat files, remove the design kp of the survey and useless comments.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD02B486-BE51-4277-9279-B2A8299B764C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0056F324-9A42-40B8-858F-B9AAFB03E6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,13 @@
     <sheet name="Legend" sheetId="3" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BlockJoint!$A$4:$J$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Buffer!$A$4:$J$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">FloodGate!$A$4:$J$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Platform!$A$4:$J$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Signal!$A$4:$J$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Switch!$A$4:$J$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Tag!$A$4:$J$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BlockJoint!$A$4:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Buffer!$A$4:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">FloodGate!$A$4:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Platform!$A$4:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Signal!$A$4:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Switch!$A$4:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Tag!$A$4:$I$4</definedName>
     <definedName name="buffer_tol">Buffer!$B$1</definedName>
     <definedName name="flood_gate_tol">FloodGate!$B$1</definedName>
     <definedName name="joint_tol">BlockJoint!$B$1</definedName>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="85">
   <si>
     <t>Author</t>
   </si>
@@ -360,9 +360,6 @@
   </si>
   <si>
     <t>Surveyed KP</t>
-  </si>
-  <si>
-    <t>Design KP</t>
   </si>
   <si>
     <t>Difference</t>
@@ -990,7 +987,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1116,9 +1113,6 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1224,9 +1218,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2200,62 +2191,62 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="58"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="56"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="56"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="58"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="56"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="60"/>
     </row>
     <row r="21" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
@@ -2362,7 +2353,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2382,19 +2373,19 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="51" t="s">
         <v>83</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2498,13 +2489,13 @@
       <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="68">
+      <c r="A3" s="67">
         <v>2</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="69" t="s">
         <v>61</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -2517,9 +2508,9 @@
       <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="19" t="s">
         <v>63</v>
       </c>
@@ -2549,32 +2540,32 @@
       <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="68">
+      <c r="A6" s="67">
         <v>4</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="69" t="s">
         <v>53</v>
       </c>
       <c r="E6" s="42"/>
       <c r="F6" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
       <c r="E7" s="20"/>
       <c r="F7" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" s="32"/>
     </row>
@@ -2617,34 +2608,34 @@
       <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="68">
+      <c r="A10" s="67">
         <v>7</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="69" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="62" t="s">
+      <c r="E10" s="65"/>
+      <c r="F10" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="64"/>
+      <c r="G10" s="63"/>
     </row>
     <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="72"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="65"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="64"/>
     </row>
     <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
@@ -2792,7 +2783,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -2806,15 +2797,14 @@
     <col min="3" max="3" width="11.5703125" style="35" customWidth="1"/>
     <col min="4" max="4" width="18" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="35"/>
+    <col min="6" max="6" width="15.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>32</v>
       </c>
@@ -2825,69 +2815,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75"/>
       <c r="B4" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="74"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="7">
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="F1:G1048576">
     <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
@@ -2895,7 +2881,7 @@
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="55" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -2903,7 +2889,7 @@
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -2923,7 +2909,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -2937,17 +2923,16 @@
     <col min="3" max="3" width="11.5703125" style="35"/>
     <col min="4" max="4" width="18" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="35"/>
+    <col min="6" max="6" width="15.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="38">
         <v>6.0000000000000001E-3</v>
@@ -2956,69 +2941,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75"/>
       <c r="B4" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="74"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="7">
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="F1:G1048576">
     <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
@@ -3026,7 +3007,7 @@
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3034,7 +3015,7 @@
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3054,7 +3035,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3068,17 +3049,16 @@
     <col min="3" max="3" width="11.5703125" style="35"/>
     <col min="4" max="4" width="18" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="35"/>
+    <col min="6" max="6" width="15.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="38">
         <v>6.0000000000000001E-3</v>
@@ -3087,69 +3067,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75"/>
       <c r="B4" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="74"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <mergeCells count="7">
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="F1:G1048576">
     <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
@@ -3157,7 +3133,7 @@
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3165,7 +3141,7 @@
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3185,7 +3161,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3199,17 +3175,16 @@
     <col min="3" max="3" width="11.5703125" style="35"/>
     <col min="4" max="4" width="18" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="35"/>
+    <col min="6" max="6" width="15.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="38">
         <v>6.0000000000000001E-3</v>
@@ -3218,69 +3193,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75"/>
       <c r="B4" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="74"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <mergeCells count="7">
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="F1:G1048576">
     <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
@@ -3288,7 +3259,7 @@
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3296,7 +3267,7 @@
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3316,7 +3287,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3330,17 +3301,16 @@
     <col min="3" max="3" width="11.5703125" style="35"/>
     <col min="4" max="4" width="18" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="35"/>
+    <col min="6" max="6" width="15.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="38">
         <v>6.0000000000000001E-3</v>
@@ -3349,69 +3319,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75"/>
       <c r="B4" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="74"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
+  <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="7">
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="F1:G1048576">
     <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
@@ -3419,7 +3385,7 @@
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3427,7 +3393,7 @@
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3447,7 +3413,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3461,17 +3427,16 @@
     <col min="3" max="3" width="11.5703125" style="35"/>
     <col min="4" max="4" width="18" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="35"/>
+    <col min="6" max="6" width="15.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="38">
         <v>6.0000000000000001E-3</v>
@@ -3480,69 +3445,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75"/>
       <c r="B4" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="74"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <mergeCells count="7">
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="F1:G1048576">
     <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
@@ -3550,7 +3511,7 @@
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3558,7 +3519,7 @@
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3578,11 +3539,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3592,17 +3553,16 @@
     <col min="3" max="3" width="11.5703125" style="35"/>
     <col min="4" max="4" width="18" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="35"/>
+    <col min="6" max="6" width="15.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="38">
         <v>6.0000000000000001E-3</v>
@@ -3611,69 +3571,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="79" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75"/>
       <c r="B4" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="74"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <mergeCells count="7">
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="F1:G1048576">
     <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
@@ -3681,7 +3637,7 @@
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3689,7 +3645,7 @@
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>

</xml_diff>

<commit_message>
In survey verification, if center point segment "_C" does not exist in the survey, try to take the left or right point if they are on the same track. Change in the format of the result file to add borders.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9562DA-ECE3-445D-BCCA-0D3D1B774F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292E8A1-261B-4F85-BB35-3860E3658B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -407,6 +407,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -999,7 +1002,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1135,6 +1138,7 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1231,7 +1235,9 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
@@ -1242,7 +1248,937 @@
     <cellStyle name="Normal 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 6 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="181">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2203,62 +3139,62 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="56"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="56"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="57"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="60"/>
     </row>
     <row r="21" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
@@ -2396,39 +3332,39 @@
       <c r="A5" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="51" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="2" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="3" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="125" priority="4" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="KO">
+    <cfRule type="containsText" dxfId="124" priority="5" operator="containsText" text="KO">
       <formula>NOT(ISERROR(SEARCH("KO",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="123" priority="6" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="122" priority="7" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="9" stopIfTrue="1" operator="equal">
       <formula>"NOK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2499,13 +3435,13 @@
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="66">
+      <c r="A3" s="67">
         <v>2</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -2518,9 +3454,9 @@
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="16" t="s">
         <v>61</v>
       </c>
@@ -2550,16 +3486,16 @@
       <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="66">
+      <c r="A6" s="67">
         <v>4</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="69" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="39"/>
@@ -2569,10 +3505,10 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="67"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
       <c r="E7" s="17"/>
       <c r="F7" s="38" t="s">
         <v>73</v>
@@ -2620,34 +3556,34 @@
       <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="66">
+      <c r="A10" s="67">
         <v>7</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="69" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="64"/>
-      <c r="F10" s="60" t="s">
+      <c r="E10" s="65"/>
+      <c r="F10" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="62"/>
+      <c r="G10" s="63"/>
     </row>
     <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="63"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="64"/>
     </row>
     <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
@@ -2761,13 +3697,13 @@
     <mergeCell ref="D6:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="3" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2809,8 +3745,8 @@
     <col min="3" max="3" width="11.5703125" style="32" customWidth="1"/>
     <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="32"/>
@@ -2826,37 +3762,38 @@
       <c r="C1" s="34" t="s">
         <v>32</v>
       </c>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -2869,10 +3806,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="72"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -2885,30 +3822,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="cellIs" dxfId="177" priority="12" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="13" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="55" priority="6" operator="equal">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="cellIs" dxfId="175" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="15" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="9" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="10" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="11" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2935,8 +3888,8 @@
     <col min="3" max="3" width="11.5703125" style="32"/>
     <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="32"/>
@@ -2952,37 +3905,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -2995,10 +3949,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="72"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3011,30 +3965,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="cellIs" dxfId="170" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="20" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="cellIs" dxfId="168" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="22" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="18" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3061,8 +4031,8 @@
     <col min="3" max="3" width="11.5703125" style="32"/>
     <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="32"/>
@@ -3078,37 +4048,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -3121,10 +4092,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="72"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -3137,30 +4108,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="cellIs" dxfId="163" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="20" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="cellIs" dxfId="161" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="22" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="18" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3187,8 +4174,8 @@
     <col min="3" max="3" width="11.5703125" style="32"/>
     <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="32"/>
@@ -3204,37 +4191,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -3247,10 +4235,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="72"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -3263,30 +4251,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="cellIs" dxfId="156" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="20" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="cellIs" dxfId="154" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="22" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="18" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3313,8 +4317,8 @@
     <col min="3" max="3" width="11.5703125" style="32"/>
     <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="32"/>
@@ -3330,37 +4334,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -3373,10 +4378,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="72"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -3389,30 +4394,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="cellIs" dxfId="149" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="20" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="cellIs" dxfId="147" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="22" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="18" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3439,8 +4460,8 @@
     <col min="3" max="3" width="11.5703125" style="32"/>
     <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="32"/>
@@ -3456,37 +4477,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -3499,10 +4521,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="72"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -3515,30 +4537,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="cellIs" dxfId="142" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="20" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="cellIs" dxfId="140" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="22" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="18" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3565,8 +4603,8 @@
     <col min="3" max="3" width="11.5703125" style="32"/>
     <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="32"/>
@@ -3582,37 +4620,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -3625,10 +4664,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="72"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
@@ -3641,30 +4680,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="cellIs" dxfId="135" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="20" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="cellIs" dxfId="133" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="22" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="18" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add a global README. Add more information to the Survey Verification README. Modify the survey template.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292E8A1-261B-4F85-BB35-3860E3658B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E63C62-7A53-46BD-9198-57763F16D1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="85">
   <si>
     <t>Author</t>
   </si>
@@ -1139,6 +1139,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1234,9 +1237,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1248,937 +1248,7 @@
     <cellStyle name="Normal 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 6 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="181">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="68">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2329,11 +1399,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color rgb="FF9C0006"/>
@@ -2341,8 +1406,19 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2388,11 +1464,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2403,8 +1474,19 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2450,11 +1532,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2465,8 +1542,19 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2512,11 +1600,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2527,8 +1610,19 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2574,11 +1668,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2589,8 +1678,19 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2636,11 +1736,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2651,8 +1746,19 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2698,16 +1804,22 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
     </dxf>
     <dxf>
       <font>
         <b/>
         <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -3139,62 +2251,62 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="58"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="57"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="55"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="57"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="55"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="57"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="58"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="58"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="61"/>
     </row>
     <row r="21" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
@@ -3338,33 +2450,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="128" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="125" priority="4" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="5" operator="containsText" text="KO">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="KO">
       <formula>NOT(ISERROR(SEARCH("KO",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="6" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="7" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" stopIfTrue="1" operator="equal">
       <formula>"NOK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3435,13 +2547,13 @@
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="67">
+      <c r="A3" s="68">
         <v>2</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="70" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -3454,9 +2566,9 @@
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="16" t="s">
         <v>61</v>
       </c>
@@ -3486,16 +2598,16 @@
       <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="67">
+      <c r="A6" s="68">
         <v>4</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="70" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="39"/>
@@ -3505,10 +2617,10 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="17"/>
       <c r="F7" s="38" t="s">
         <v>73</v>
@@ -3556,34 +2668,36 @@
       <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="67">
+      <c r="A10" s="68">
         <v>7</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="65"/>
-      <c r="F10" s="61" t="s">
+      <c r="E10" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="63"/>
+      <c r="G10" s="64"/>
     </row>
     <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="64"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="65"/>
     </row>
     <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
@@ -3598,7 +2712,9 @@
       <c r="D12" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="24"/>
+      <c r="E12" s="24" t="s">
+        <v>74</v>
+      </c>
       <c r="F12" s="22" t="s">
         <v>36</v>
       </c>
@@ -3697,13 +2813,13 @@
     <mergeCell ref="D6:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3762,38 +2878,38 @@
       <c r="C1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="84"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="73" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -3806,10 +2922,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -3822,46 +2938,37 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:G1048576">
-    <cfRule type="cellIs" dxfId="177" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="12" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="13" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="175" priority="14" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="173" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="11" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="11" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3905,38 +3012,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="84"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="73" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -3949,10 +3056,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3965,46 +3072,37 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:G1048576">
-    <cfRule type="cellIs" dxfId="170" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="20" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="168" priority="21" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="166" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="18" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="18" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4048,38 +3146,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="84"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="73" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -4092,10 +3190,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -4108,46 +3206,37 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:G1048576">
-    <cfRule type="cellIs" dxfId="163" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="20" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="161" priority="21" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="159" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="18" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="18" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4191,38 +3280,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="84"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="73" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -4235,10 +3324,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -4251,46 +3340,37 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:G1048576">
-    <cfRule type="cellIs" dxfId="156" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="20" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="154" priority="21" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="152" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="18" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="18" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4334,38 +3414,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="84"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="73" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -4378,10 +3458,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -4394,46 +3474,37 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:G1048576">
-    <cfRule type="cellIs" dxfId="149" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="20" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="147" priority="21" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="145" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="18" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4477,38 +3548,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="84"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="73" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -4521,10 +3592,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -4537,46 +3608,37 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:G1048576">
-    <cfRule type="cellIs" dxfId="142" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="20" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="140" priority="21" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="138" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="18" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4620,38 +3682,38 @@
       <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="84"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="73" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -4664,10 +3726,10 @@
       <c r="E4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
@@ -4680,46 +3742,37 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+      <formula>"Not in DC_SYS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:G1048576">
-    <cfRule type="cellIs" dxfId="135" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="20" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="133" priority="21" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="131" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="18" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Not in DC_SYS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update DC_TU verification and survey verification result files. Add a function to get direction of oriented points and update functions point in zone accordingly. Add verification of message type vital/non vital for General Data. Updates in ZC-IXL interface to do constraints for 6.6. Some change in CF_SIGNAL_12 to be able to read as input an IXL APZ file (still to update function to compute the IXL APZ by default (the IVB of the signal) and to be able to change this to take the first CDV as what is done on Milan and TSK. Change survey verif to take as key object_name+track, there was issues on Milan where multiple joints have the same name in survey file.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E63C62-7A53-46BD-9198-57763F16D1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76F013B-8A52-49D7-8C4C-9BBA02A6BF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -2501,7 +2501,7 @@
     <col min="4" max="4" width="49.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="108.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Small fixes in Survey Verification. Rework of interface ZC-IXL Verification, still TODO to do. Rework of CF_SIGNAL_12 verif, now we can select between IVB and TC Approach Zone, and use a file in input only for a few signals.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76F013B-8A52-49D7-8C4C-9BBA02A6BF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB4257-E1EF-49DD-B0B8-DFCD4697E569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -1002,7 +1002,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1076,12 +1076,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1176,12 +1170,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1237,6 +1225,27 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2251,62 +2260,62 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="58"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="56"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="56"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="58"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="56"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
     </row>
     <row r="21" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
@@ -2339,9 +2348,9 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
       <c r="F24"/>
       <c r="G24"/>
     </row>
@@ -2365,21 +2374,21 @@
       <c r="C27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="49"/>
+      <c r="D27" s="47"/>
       <c r="E27"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="47"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="50"/>
+      <c r="D29" s="48"/>
       <c r="E29"/>
     </row>
   </sheetData>
@@ -2433,18 +2442,18 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="44" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="49" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2501,7 +2510,7 @@
     <col min="4" max="4" width="49.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="108.140625" customWidth="1"/>
+    <col min="7" max="7" width="108.140625" style="87" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2541,34 +2550,34 @@
         <v>62</v>
       </c>
       <c r="E2" s="17"/>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="30"/>
+      <c r="G2" s="81"/>
     </row>
     <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="68">
+      <c r="A3" s="64">
         <v>2</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="66" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>60</v>
       </c>
       <c r="E3" s="19"/>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="82"/>
     </row>
     <row r="4" spans="1:7" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="16" t="s">
         <v>61</v>
       </c>
@@ -2576,7 +2585,7 @@
       <c r="F4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="29"/>
+      <c r="G4" s="83"/>
     </row>
     <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
@@ -2592,40 +2601,40 @@
         <v>50</v>
       </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="83"/>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="68">
+      <c r="A6" s="64">
         <v>4</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="82"/>
     </row>
     <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
       <c r="E7" s="17"/>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
@@ -2644,7 +2653,7 @@
       <c r="F8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="29"/>
+      <c r="G8" s="83"/>
     </row>
     <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
@@ -2665,39 +2674,39 @@
       <c r="F9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="84"/>
     </row>
     <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="68">
+      <c r="A10" s="64">
         <v>7</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="66" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="64"/>
+      <c r="G10" s="85"/>
     </row>
     <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="72"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="65"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
@@ -2718,7 +2727,7 @@
       <c r="F12" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="84"/>
     </row>
     <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
@@ -2734,10 +2743,10 @@
         <v>56</v>
       </c>
       <c r="E13" s="17"/>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="29"/>
+      <c r="G13" s="83"/>
     </row>
     <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
@@ -2753,10 +2762,10 @@
         <v>56</v>
       </c>
       <c r="E14" s="17"/>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="83"/>
     </row>
     <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
@@ -2772,10 +2781,10 @@
         <v>57</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="29"/>
+      <c r="G15" s="83"/>
     </row>
     <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
@@ -2794,7 +2803,7 @@
       <c r="F16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="29"/>
+      <c r="G16" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2856,76 +2865,76 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="33"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -2990,76 +2999,76 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32"/>
-    <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="30"/>
+    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="33"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3124,76 +3133,76 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32"/>
-    <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="30"/>
+    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="33"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -3258,76 +3267,76 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32"/>
-    <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="30"/>
+    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="33"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -3392,76 +3401,76 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32"/>
-    <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="30"/>
+    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="33"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -3526,76 +3535,76 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32"/>
-    <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="30"/>
+    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="33"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -3660,76 +3669,76 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32"/>
-    <col min="4" max="4" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="30"/>
+    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="33"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
Modify survey template to adapt to versions after 7.2.0.0 with a line for PSD. Change the way to get GA version, in order to print the info and check here if version is older than 7.2.0.0 to delete the associated line in the survey template.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB4257-E1EF-49DD-B0B8-DFCD4697E569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C36F4D-0FCC-4521-8F3B-AC5C93A80612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="89">
   <si>
     <t>Author</t>
   </si>
@@ -163,9 +163,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>M:</t>
-  </si>
-  <si>
     <t>A: Sheet "Switch"</t>
   </si>
   <si>
@@ -179,90 +176,6 @@
   </si>
   <si>
     <t>A: Sheet "FloodGate"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER] 
-Flood Gate topographic measures
-[ADONF] data:
--Flood_Gate [Name], [Limit] &lt; [Segment, offset, Direction]&gt;, [Blocks]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER] 
-Anchor topographic measures
-[ADONF] data:
--Anchor [Surveyed KP]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-Tags topographic measures
- [ADONF] data:
-- Dynamic Tag [Stop_Signal], [Type], [Route List]:[Route Name], [Vital Stopping Point]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-Tags topographic measures 
-[ADONF] data:
-- Localization Tag [Tag Name], [offset, Seg]
-- Segment [Direction]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consistency between Directional Permanent Speed Restriction [Directional Permanent Speed Restriction Limits] &lt;[Segment, Offset]&gt; and[Directional Permanent Speed Restriction Limits] &lt;[Anticipation Distance]&gt; and Topographic measures:
-- KP conversions and comparison with topographic measures
-If [Anticipation Distance] &lt;&gt; 0 then KP comparisons with topographic measures has to account this distance
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-Directional Speed limit topographic measures 
-[ADONF] data:
-- Directional Permanent Speed Restriction [Speed value], [Direction], [Directional Permanent Speed Restriction Limits]: [offset, Seg],[Directional Permanent Speed Restriction Limits]: [Anticipation Distance]
-- Segment [Name], [Origin KP], [Direction]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-Speed limit topographic measures
-[ADONF] data:
-- Permanent Speed Restriction [Speed value], [Permanent Speed Restriction Limits]: [offset, Seg],[Permanent Speed Restriction Limits]: [Anticipation Distance]
-- Segment [Name], [Origin KP], [Direction]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-Slope profile topographic measures 
-[ADONF] data:
--  Slope Profile [Segment, offset],[Slope Value]
-- Segment [Names, [Origin KP], [Direction]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-DD topographic measures
-[ADONF] data:
-- Discrete Detector [offset, Seg]
-- Segment [Name], [Origin PK], [Direction]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-Signals topographic measures
-[ADONF] data: 
-- Line [Referential]
-- Signals [offset, Seg], [Direction], [Type]
-- Segment [Name], [Origin KP], [Direction]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CUSTOMER]
-Block topographic measures
-[ADONF] data:
-- Block [Limit List] : [offset, Seg]
-- Segment [Name], [Origin KP], [Direction]
-</t>
   </si>
   <si>
     <t xml:space="preserve">KP conversion and comparison with Block topographic measures. 
@@ -285,12 +198,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Consistency between Permanent Speed Restriction [Permanent Speed Restriction Limits] &lt;[Segment, Offset]&gt; and[Permanent Speed Restriction Limits] &lt;[Anticipation Distance]&gt; and topographic measures:
-- KP conversions and comparison with topographic measures 
-If [Anticipation Distance] &lt;&gt; 0 then KP comparisons with topographic measures has to account this distance.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">KP conversion of tag position and comparison with tags topographic measures.
 </t>
   </si>
@@ -299,108 +206,219 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">KP Anchor position and comparison with assiociated objects topographic measures.
+    <t xml:space="preserve">Check consistency between KP over the 3 switches components on the switch point.
+</t>
+  </si>
+  <si>
+    <t>Data Name</t>
+  </si>
+  <si>
+    <t>DC_SYS</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>KP</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>Surveyed KP</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Manual Verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Sheet "Signal"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Sheet "Buffer"
+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Signification</t>
+  </si>
+  <si>
+    <t>Tolerance on platform ends location:</t>
+  </si>
+  <si>
+    <t>Tolerance on switches location:</t>
+  </si>
+  <si>
+    <t>Tolerance on joints location:</t>
+  </si>
+  <si>
+    <t>Tolerance on signals location:</t>
+  </si>
+  <si>
+    <t>Tolerance on buffers location:</t>
+  </si>
+  <si>
+    <t>Tolerance on tags location:</t>
+  </si>
+  <si>
+    <t>Tolerance on flood gates location:</t>
+  </si>
+  <si>
+    <t>A: Sheet "Block_Joint"</t>
+  </si>
+  <si>
+    <t>The name of the survey is different from the one expected by the tool. So line is duplicated with the one generated from the DC_SYS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP Anchor position and comparison with associated objects topographic measures.
 Check for each track: 
 - that the Surveyed KP of each anchor corresponds to the KP of an object surveyed in D932.
 - that the Civil KP  of each anchor corresponds to the KP of an object mentioned in the signal plan.
 </t>
   </si>
   <si>
+    <t>PSD</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CUSTOMER] 
+PSD measures
+[CBTC_DB]: DC_SYS.xls data:
+- OSP platform related
+- PSD subset
+- TD subset
+- Authorized consists at OSP
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CUSTOMER]
+Tags topographic measures
+ [CBTC_DB]: DC_SYS.xls data:
+- Dynamic Tag [Stop_Signal], [Type], [Route List]:[Route Name], [Vital Stopping Point]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CUSTOMER] 
+Anchor topographic measures
+[CBTC_DB]: DC_SYS.xls data:
+- Anchor [Surveyed KP]
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">[CUSTOMER]
 Platform ends topographic measures
 Operational Stopping Point topographic measures
-[ADONF] data:
+[CBTC_DB]: DC_SYS.xls data:
 - Platform [Station name]
 - Platform ends [KP, Seg]
 - Segment [Name], [Origin KP], [Direction]
 - Line [Reference Segment]
-- Operational Stopping Point [offset, Seg] 
+- Operational Stopping Point [Offset, Seg] 
 - Segment [Name], [Origin KP], [Direction]
 </t>
   </si>
   <si>
-    <t xml:space="preserve">KP Conversion and platform ends comparison with topographic measures
+    <t xml:space="preserve">[CUSTOMER]
+[CBTC_DB]: DC_SYS.xls data:
+- Segment [Track Name], [Origin KP], [End KP]
+- Switch [Point Segment Name], [Left Heel Segment Name], [Right Heel Segment Name]
 </t>
   </si>
   <si>
-    <t xml:space="preserve">KP conversion and comparison between Operational Stopping Point and Operational Stopping Point Topographic measures.
+    <t xml:space="preserve">[CUSTOMER]
+Block topographic measures
+[CBTC_DB]: DC_SYS.xls data:
+- Block [Limit List] : [Offset, Seg]
+- Segment [Name], [Origin KP], [Direction]
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Check consistency between KP over the 3 switches components on the switch point.
+    <t xml:space="preserve">[CUSTOMER]
+Signals topographic measures
+[CBTC_DB]: DC_SYS.xls data: 
+- Line [Referential]
+- Signals [Offset, Seg], [Direction], [Type]
+- Segment [Name], [Origin KP], [Direction]
 </t>
   </si>
   <si>
     <t xml:space="preserve">[CUSTOMER]
-[ADONF] data:
-- Segment [Track Name], [Orig KP], [end KP]
-- Switch[Point Segment Name], [Left Heel Segment Name], [Right Heel Segment Name]
+DD topographic measures
+[CBTC_DB]: DC_SYS.xls data:
+- Discrete Detector [Offset, Seg]
+- Segment [Name], [Origin PK], [Direction]
 </t>
   </si>
   <si>
-    <t>Data Name</t>
-  </si>
-  <si>
-    <t>DC_SYS</t>
-  </si>
-  <si>
-    <t>Track</t>
-  </si>
-  <si>
-    <t>KP</t>
-  </si>
-  <si>
-    <t>Survey</t>
-  </si>
-  <si>
-    <t>Surveyed KP</t>
-  </si>
-  <si>
-    <t>Difference</t>
-  </si>
-  <si>
-    <t>Manual Verification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A: Sheet "Signal"
+    <t xml:space="preserve">[CUSTOMER]
+Slope profile topographic measures 
+[CBTC_DB]: DC_SYS.xls data:
+- Slope Profile [Segment, Offset], [Slope Value]
+- Segment [Name], [Origin KP], [Direction]
 </t>
   </si>
   <si>
-    <t xml:space="preserve">A: Sheet "Buffer"
+    <t xml:space="preserve">[CUSTOMER]
+Speed limit topographic measures
+[CBTC_DB]: DC_SYS.xls data:
+- Permanent Speed Restriction [Speed Value], [Permanent Speed Restriction Limits]: [Offset, Seg], [Permanent Speed Restriction Limits]: [Anticipation Distance]
+- Segment [Name], [Origin KP], [Direction]
 </t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Signification</t>
-  </si>
-  <si>
-    <t>Tolerance on platform ends location:</t>
-  </si>
-  <si>
-    <t>Tolerance on switches location:</t>
-  </si>
-  <si>
-    <t>Tolerance on joints location:</t>
-  </si>
-  <si>
-    <t>Tolerance on signals location:</t>
-  </si>
-  <si>
-    <t>Tolerance on buffers location:</t>
-  </si>
-  <si>
-    <t>Tolerance on tags location:</t>
-  </si>
-  <si>
-    <t>Tolerance on flood gates location:</t>
-  </si>
-  <si>
-    <t>A: Sheet "Block_Joint"</t>
-  </si>
-  <si>
-    <t>The name of the survey is different from the one expected by the tool. So line is duplicated with the one generated from the DC_SYS.</t>
+    <t xml:space="preserve">[CUSTOMER]
+Directional Speed limit topographic measures 
+[CBTC_DB]: DC_SYS.xls data:
+- Directional Permanent Speed Restriction [Speed Value], [Direction], [Directional Permanent Speed Restriction Limits]: [Offset, Seg], [Directional Permanent Speed Restriction Limits]: [Anticipation Distance]
+- Segment [Name], [Origin KP], [Direction]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CUSTOMER]
+Tags topographic measures 
+[CBTC_DB]: DC_SYS.xls data:
+- Localization Tag [Tag Name], [Offset, Seg]
+- Segment [Direction]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CUSTOMER] 
+Flood Gate topographic measures
+[CBTC_DB]: DC_SYS.xls data:
+- Flood_Gate [Name], [Limit] &lt;[Segment, Offset, Direction]&gt;, [Blocks]
+</t>
+  </si>
+  <si>
+    <t>M: Check with Data Preparation Need Specification and D932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSD check position.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consistency between Permanent Speed Restriction [Permanent Speed Restriction Limits] &lt;[Segment, Offset]&gt; and [Permanent Speed Restriction Limits] &lt;[Anticipation Distance]&gt; and topographic measures:
+- KP conversions and comparison with topographic measures.
+If [Anticipation Distance] &lt;&gt; 0 then KP comparisons with topographic measures has to account this distance.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consistency between Directional Permanent Speed Restriction [Directional Permanent Speed Restriction Limits] &lt;[Segment, Offset]&gt; and [Directional Permanent Speed Restriction Limits] &lt;[Anticipation Distance]&gt; and Topographic measures:
+- KP conversions and comparison with topographic measures.
+If [Anticipation Distance] &lt;&gt; 0 then KP comparisons with topographic measures has to account this distance.
+</t>
+  </si>
+  <si>
+    <t>KP conversion and comparison between Operational Stopping Point and Operational Stopping Point topographic measures.</t>
+  </si>
+  <si>
+    <t>KP Conversion and platform ends comparison with topographic measures.</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1020,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1038,13 +1056,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1052,30 +1064,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1091,20 +1085,8 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="18" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1136,6 +1118,33 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1170,6 +1179,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1182,10 +1197,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1226,26 +1241,23 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="18" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2237,94 +2249,94 @@
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="2" width="16.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-    </row>
-    <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="56"/>
-    </row>
-    <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="56"/>
-    </row>
-    <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="57"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
-    </row>
-    <row r="21" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="51"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="53"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53"/>
+    </row>
+    <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="51"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="53"/>
+    </row>
+    <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="53"/>
+    </row>
+    <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="51"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="53"/>
+    </row>
+    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="2:7" ht="21" x14ac:dyDescent="0.4">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
@@ -2332,7 +2344,7 @@
       <c r="F22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23"/>
       <c r="C23" s="5" t="s">
         <v>0</v>
@@ -2346,15 +2358,15 @@
       <c r="F23"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
       <c r="F24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -2362,7 +2374,7 @@
       <c r="F25"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -2370,25 +2382,25 @@
       <c r="F26"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="47"/>
+      <c r="D27" s="35"/>
       <c r="E27"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C28" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="47"/>
+      <c r="D28" s="35"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="48"/>
+      <c r="D29" s="36"/>
       <c r="E29"/>
     </row>
   </sheetData>
@@ -2410,22 +2422,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="10"/>
-    <col min="2" max="2" width="121.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5703125" style="10"/>
+    <col min="1" max="1" width="11.5546875" style="10"/>
+    <col min="2" max="2" width="121.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -2433,7 +2445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -2441,20 +2453,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>84</v>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2498,22 +2510,25 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="108.140625" style="87" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="85" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="44" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="85" customWidth="1"/>
+    <col min="6" max="6" width="30" style="44" customWidth="1"/>
+    <col min="7" max="7" width="108.109375" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -2536,274 +2551,293 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="34" t="s">
+      <c r="C2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="63">
+        <v>2</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="81"/>
-    </row>
-    <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="64">
-        <v>2</v>
-      </c>
-      <c r="B3" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="82"/>
-    </row>
-    <row r="4" spans="1:7" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="83"/>
-    </row>
-    <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="40"/>
+    </row>
+    <row r="4" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="64"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="83"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="64">
+      <c r="C5" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="41"/>
+    </row>
+    <row r="6" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="63">
         <v>4</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="82"/>
-    </row>
-    <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="65"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="83"/>
-    </row>
-    <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="40"/>
+    </row>
+    <row r="7" spans="1:7" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="64"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="41"/>
+    </row>
+    <row r="8" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="83"/>
-    </row>
-    <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="84"/>
-    </row>
-    <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="64">
+      <c r="C9" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="42"/>
+    </row>
+    <row r="10" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="63">
         <v>7</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="85"/>
-    </row>
-    <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="68"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="86"/>
-    </row>
-    <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="59"/>
+    </row>
+    <row r="11" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="67"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="62"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="60"/>
+    </row>
+    <row r="12" spans="1:7" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <v>8</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="84"/>
-    </row>
-    <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="42"/>
+    </row>
+    <row r="13" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="83"/>
-    </row>
-    <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="41"/>
+    </row>
+    <row r="14" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <v>10</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="83"/>
-    </row>
-    <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <v>11</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="83"/>
-    </row>
-    <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>12</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="83"/>
+      <c r="C16" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="83" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15">
+        <v>13</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2833,7 +2867,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10 E12:E16" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10 E12:E17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"KO, OK, NA, -"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2863,78 +2897,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="33">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="77" t="s">
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="70"/>
+      <c r="I3" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -2997,78 +3031,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="30"/>
-    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="22"/>
+    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="33">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="77" t="s">
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="70"/>
+      <c r="I3" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3131,78 +3165,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="30"/>
-    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="22"/>
+    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="33">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="77" t="s">
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="70"/>
+      <c r="I3" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -3265,78 +3299,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="30"/>
-    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="22"/>
+    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="33">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="77" t="s">
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="70"/>
+      <c r="I3" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -3399,78 +3433,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="30"/>
-    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="22"/>
+    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="33">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="77" t="s">
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="70"/>
+      <c r="I3" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -3533,78 +3567,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="30"/>
-    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="22"/>
+    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="33">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="77" t="s">
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="70"/>
+      <c r="I3" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -3667,78 +3701,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="30"/>
-    <col min="4" max="4" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="22"/>
+    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="33">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="77" t="s">
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="70"/>
+      <c r="I3" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
Fixes in survey verification. Adapt to work on more projects (Lima, Riyadh, NMML1).
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C36F4D-0FCC-4521-8F3B-AC5C93A80612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D28062-7570-4713-954C-CDB03BF6BE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1145,6 +1145,24 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="18" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1240,24 +1258,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="18" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2272,62 +2272,62 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="59"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="59"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="51"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="59"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="2:7" ht="21" x14ac:dyDescent="0.4">
       <c r="B21" s="4"/>
@@ -2519,11 +2519,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="85" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="53" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.109375" style="44" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" style="44" customWidth="1"/>
     <col min="4" max="4" width="49.88671875" style="44" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="85" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="53" customWidth="1"/>
     <col min="6" max="6" width="30" style="44" customWidth="1"/>
     <col min="7" max="7" width="108.109375" style="44" customWidth="1"/>
   </cols>
@@ -2565,34 +2565,34 @@
         <v>45</v>
       </c>
       <c r="E2" s="16"/>
-      <c r="F2" s="80" t="s">
+      <c r="F2" s="48" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63">
+      <c r="A3" s="69">
         <v>2</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="71" t="s">
         <v>73</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>88</v>
       </c>
       <c r="E3" s="17"/>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="49" t="s">
         <v>34</v>
       </c>
       <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="64"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="20" t="s">
         <v>87</v>
       </c>
@@ -2616,37 +2616,37 @@
         <v>38</v>
       </c>
       <c r="E5" s="16"/>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="50" t="s">
         <v>65</v>
       </c>
       <c r="G5" s="41"/>
     </row>
     <row r="6" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63">
+      <c r="A6" s="69">
         <v>4</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="71" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="26"/>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="49" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:7" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="64"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="82" t="s">
+      <c r="F7" s="50" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="41"/>
@@ -2665,7 +2665,7 @@
         <v>40</v>
       </c>
       <c r="E8" s="16"/>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="51" t="s">
         <v>69</v>
       </c>
       <c r="G8" s="41"/>
@@ -2686,42 +2686,42 @@
       <c r="E9" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="83" t="s">
+      <c r="F9" s="51" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="63">
+      <c r="A10" s="69">
         <v>7</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="71" t="s">
         <v>79</v>
       </c>
       <c r="D10" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="59"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="67"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="60"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="66"/>
     </row>
     <row r="12" spans="1:7" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
@@ -2739,7 +2739,7 @@
       <c r="E12" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="83" t="s">
+      <c r="F12" s="51" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="42"/>
@@ -2758,7 +2758,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="16"/>
-      <c r="F13" s="84" t="s">
+      <c r="F13" s="52" t="s">
         <v>36</v>
       </c>
       <c r="G13" s="41"/>
@@ -2777,7 +2777,7 @@
         <v>43</v>
       </c>
       <c r="E14" s="16"/>
-      <c r="F14" s="84" t="s">
+      <c r="F14" s="52" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="41"/>
@@ -2796,7 +2796,7 @@
         <v>44</v>
       </c>
       <c r="E15" s="16"/>
-      <c r="F15" s="84" t="s">
+      <c r="F15" s="52" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="41"/>
@@ -2815,7 +2815,7 @@
         <v>67</v>
       </c>
       <c r="E16" s="16"/>
-      <c r="F16" s="83" t="s">
+      <c r="F16" s="51" t="s">
         <v>83</v>
       </c>
       <c r="G16" s="41"/>
@@ -2834,7 +2834,7 @@
         <v>84</v>
       </c>
       <c r="E17" s="16"/>
-      <c r="F17" s="83" t="s">
+      <c r="F17" s="51" t="s">
         <v>69</v>
       </c>
       <c r="G17" s="41"/>
@@ -2927,32 +2927,32 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="74" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="27" t="s">
         <v>48</v>
       </c>
@@ -2965,10 +2965,10 @@
       <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -3027,7 +3027,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -3061,32 +3061,32 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="74" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="27" t="s">
         <v>48</v>
       </c>
@@ -3099,10 +3099,10 @@
       <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3195,32 +3195,32 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="74" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="27" t="s">
         <v>48</v>
       </c>
@@ -3233,10 +3233,10 @@
       <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -3329,32 +3329,32 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="74" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="27" t="s">
         <v>48</v>
       </c>
@@ -3367,10 +3367,10 @@
       <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -3463,32 +3463,32 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="74" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="27" t="s">
         <v>48</v>
       </c>
@@ -3501,10 +3501,10 @@
       <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -3597,32 +3597,32 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="74" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="27" t="s">
         <v>48</v>
       </c>
@@ -3635,10 +3635,10 @@
       <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -3731,32 +3731,32 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="74" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="27" t="s">
         <v>48</v>
       </c>
@@ -3769,10 +3769,10 @@
       <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
Add in the header file of Survey Verification file the tool version.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D28062-7570-4713-954C-CDB03BF6BE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F1B77D-4E42-4315-9B70-828C7AFB82DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
   <si>
     <t>Author</t>
   </si>
@@ -420,6 +420,12 @@
   <si>
     <t>KP Conversion and platform ends comparison with topographic measures.</t>
   </si>
+  <si>
+    <t>v1_4</t>
+  </si>
+  <si>
+    <t>Survey_Verification_Tool:</t>
+  </si>
 </sst>
 </file>
 
@@ -428,19 +434,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -479,32 +478,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color indexed="10"/>
-      <name val="Franklin Gothic Medium"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -514,24 +487,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -550,10 +505,98 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="20"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1013,63 +1056,26 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1082,183 +1088,224 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="18" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
@@ -1909,9 +1956,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1139190</xdr:colOff>
+      <xdr:colOff>746984</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>177165</xdr:rowOff>
+      <xdr:rowOff>154753</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2243,165 +2290,174 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A6:G29"/>
+  <dimension ref="A6:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="16.33203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="2" width="16.28515625" style="83" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="83" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="83" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="83" customWidth="1"/>
+    <col min="6" max="7" width="16.28515625" style="83" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="83"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="54" t="s">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="84"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="85"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="57"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-    </row>
-    <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="57"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-    </row>
-    <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="57"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="59"/>
-    </row>
-    <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="57"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="60"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62"/>
-    </row>
-    <row r="21" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23"/>
-      <c r="C23" s="5" t="s">
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+    </row>
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="87"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+    </row>
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="87"/>
+      <c r="C23" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F23"/>
-      <c r="G23"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24"/>
-      <c r="G24"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C27" s="6" t="s">
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+    </row>
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="87"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+    </row>
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="87"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+    </row>
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C28" s="7" t="s">
+      <c r="D27" s="48"/>
+      <c r="E27" s="87"/>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C29" s="6" t="s">
+      <c r="D28" s="48"/>
+      <c r="E28" s="87"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="87"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2422,50 +2478,50 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="10"/>
-    <col min="2" max="2" width="121.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5546875" style="10"/>
+    <col min="1" max="1" width="11.5703125" style="3"/>
+    <col min="2" max="2" width="121.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="18" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2517,327 +2573,328 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" style="44" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" style="44" customWidth="1"/>
-    <col min="4" max="4" width="49.88671875" style="44" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="53" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="44" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="44" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="43" customWidth="1"/>
     <col min="6" max="6" width="30" style="44" customWidth="1"/>
-    <col min="7" max="7" width="108.109375" style="44" customWidth="1"/>
+    <col min="7" max="7" width="108.140625" style="44" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15">
+    <row r="2" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="39"/>
-    </row>
-    <row r="3" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69">
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="66">
         <v>2</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="49" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="40"/>
-    </row>
-    <row r="4" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="70"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="20" t="s">
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" ht="77.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="45" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="41"/>
-    </row>
-    <row r="5" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15">
+      <c r="G4" s="31"/>
+    </row>
+    <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="50" t="s">
+      <c r="E5" s="25"/>
+      <c r="F5" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="41"/>
-    </row>
-    <row r="6" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="69">
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="1:7" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="66">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="49" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="40"/>
-    </row>
-    <row r="7" spans="1:7" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="70"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="50" t="s">
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" ht="52.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="67"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="41"/>
-    </row>
-    <row r="8" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15">
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23">
         <v>5</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="51" t="s">
+      <c r="E8" s="25"/>
+      <c r="F8" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="41"/>
-    </row>
-    <row r="9" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
         <v>6</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="42"/>
-    </row>
-    <row r="10" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="69">
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="66">
         <v>7</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="67" t="s">
+      <c r="E10" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="65"/>
-    </row>
-    <row r="11" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="73"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="42" t="s">
+      <c r="G10" s="62"/>
+    </row>
+    <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="70"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="68"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="66"/>
-    </row>
-    <row r="12" spans="1:7" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15">
+      <c r="E11" s="65"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="63"/>
+    </row>
+    <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23">
         <v>8</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="42"/>
-    </row>
-    <row r="13" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15">
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23">
         <v>9</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="52" t="s">
+      <c r="E13" s="25"/>
+      <c r="F13" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="41"/>
-    </row>
-    <row r="14" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15">
+      <c r="G13" s="31"/>
+    </row>
+    <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23">
         <v>10</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="52" t="s">
+      <c r="E14" s="25"/>
+      <c r="F14" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="41"/>
-    </row>
-    <row r="15" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15">
+      <c r="G14" s="31"/>
+    </row>
+    <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
         <v>11</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="52" t="s">
+      <c r="E15" s="25"/>
+      <c r="F15" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="41"/>
-    </row>
-    <row r="16" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
+      <c r="G15" s="31"/>
+    </row>
+    <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23">
         <v>12</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="51" t="s">
+      <c r="E16" s="25"/>
+      <c r="F16" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="41"/>
-    </row>
-    <row r="17" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="15">
+      <c r="G16" s="31"/>
+    </row>
+    <row r="17" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23">
         <v>13</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="51" t="s">
+      <c r="E17" s="25"/>
+      <c r="F17" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="41"/>
+      <c r="G17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2897,78 +2954,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="22"/>
+    <col min="1" max="1" width="43.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="80" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="75"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -3031,78 +3088,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="22"/>
-    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="22"/>
+    <col min="1" max="1" width="43.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="80" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="75"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3165,78 +3222,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="22"/>
-    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="22"/>
+    <col min="1" max="1" width="43.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="80" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="75"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -3299,78 +3356,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="22"/>
-    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="22"/>
+    <col min="1" max="1" width="43.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="80" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="75"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -3433,78 +3490,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="22"/>
-    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="22"/>
+    <col min="1" max="1" width="43.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="80" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="75"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -3567,78 +3624,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="22"/>
-    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="22"/>
+    <col min="1" max="1" width="43.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="80" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="75"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -3701,78 +3758,78 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="22"/>
-    <col min="4" max="4" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="22"/>
+    <col min="1" max="1" width="43.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="80" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="75"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
Improve survey verification of platform. Set different colors in survey verification file for the different objects on a same sheet (tags/ IATPM_tags/IATPM_Version_Tags and platform limits/platform OSPs).
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD33D677-6C37-4256-B5AF-E6E985AB2824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDCB5A6-54D5-420C-988A-D45AEE3D5430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -435,10 +435,10 @@
     <t>Tolerance on platform OSP location:</t>
   </si>
   <si>
-    <t>v1_5</t>
-  </si>
-  <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>v1_6</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1125,6 +1125,21 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1139,7 +1154,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1292,6 +1307,12 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1352,6 +1373,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1374,15 +1404,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2375,94 +2396,94 @@
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.33203125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="49" customWidth="1"/>
-    <col min="6" max="7" width="16.33203125" style="49" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="49"/>
+    <col min="1" max="2" width="16.28515625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="49" customWidth="1"/>
+    <col min="6" max="7" width="16.28515625" style="49" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="49"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6" s="50"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58" t="s">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="61"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="63"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="63"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="61"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="63"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="61"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="63"/>
-    </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="61"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="63"/>
-    </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="61"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="63"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="62"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="65"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="65"/>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="63"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="65"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="63"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="66"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
       <c r="D21" s="53"/>
       <c r="E21" s="52"/>
       <c r="F21" s="52"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="53"/>
       <c r="C22" s="53"/>
       <c r="D22" s="53"/>
@@ -2470,7 +2491,7 @@
       <c r="F22" s="53"/>
       <c r="G22" s="53"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="53"/>
       <c r="C23" s="43" t="s">
         <v>0</v>
@@ -2484,7 +2505,7 @@
       <c r="F23" s="53"/>
       <c r="G23" s="53"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="53"/>
       <c r="C24" s="44"/>
       <c r="D24" s="44"/>
@@ -2492,7 +2513,7 @@
       <c r="F24" s="53"/>
       <c r="G24" s="53"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
       <c r="D25" s="53"/>
@@ -2500,7 +2521,7 @@
       <c r="F25" s="53"/>
       <c r="G25" s="53"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
       <c r="D26" s="53"/>
@@ -2508,30 +2529,30 @@
       <c r="F26" s="53"/>
       <c r="G26" s="53"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="45" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="46"/>
       <c r="E27" s="53"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="47" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="46"/>
       <c r="E28" s="53"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="47" t="s">
         <v>89</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E29" s="53"/>
     </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="45" t="s">
         <v>5</v>
       </c>
@@ -2557,14 +2578,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="3"/>
-    <col min="2" max="2" width="121.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5546875" style="3"/>
+    <col min="1" max="1" width="11.5703125" style="3"/>
+    <col min="2" max="2" width="121.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2572,7 +2593,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -2580,7 +2601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2588,7 +2609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
@@ -2596,7 +2617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>56</v>
       </c>
@@ -2652,19 +2673,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" style="42" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" style="42" customWidth="1"/>
-    <col min="4" max="4" width="49.88671875" style="42" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="41" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="42" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="42" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" style="42" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="41" customWidth="1"/>
     <col min="6" max="6" width="30" style="42" customWidth="1"/>
-    <col min="7" max="7" width="108.109375" style="42" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="21"/>
+    <col min="7" max="7" width="108.140625" style="42" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
@@ -2687,7 +2708,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -2706,14 +2727,14 @@
       </c>
       <c r="G2" s="26"/>
     </row>
-    <row r="3" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73">
+    <row r="3" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75">
         <v>2</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="77" t="s">
         <v>73</v>
       </c>
       <c r="D3" s="27" t="s">
@@ -2725,20 +2746,20 @@
       </c>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="74"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
+    <row r="4" spans="1:7" ht="77.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="23" t="s">
         <v>87</v>
       </c>
       <c r="E4" s="31"/>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="27"/>
-    </row>
-    <row r="5" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="59"/>
+    </row>
+    <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -2757,17 +2778,17 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="73">
+    <row r="6" spans="1:7" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
         <v>4</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="77" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="33"/>
@@ -2776,18 +2797,18 @@
       </c>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:7" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="74"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
+    <row r="7" spans="1:7" ht="52.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="76"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
       <c r="E7" s="24"/>
       <c r="F7" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="30"/>
     </row>
-    <row r="8" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -2806,7 +2827,7 @@
       </c>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -2827,39 +2848,39 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="73">
+    <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="75">
         <v>7</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="77" t="s">
         <v>79</v>
       </c>
       <c r="D10" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="71" t="s">
+      <c r="E10" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="67" t="s">
+      <c r="F10" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="69"/>
-    </row>
-    <row r="11" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="77"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
+      <c r="G10" s="71"/>
+    </row>
+    <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="79"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="72"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="70"/>
-    </row>
-    <row r="12" spans="1:7" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11" s="74"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="72"/>
+    </row>
+    <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>8</v>
       </c>
@@ -2880,7 +2901,7 @@
       </c>
       <c r="G12" s="37"/>
     </row>
-    <row r="13" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>9</v>
       </c>
@@ -2899,7 +2920,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>10</v>
       </c>
@@ -2918,7 +2939,7 @@
       </c>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>11</v>
       </c>
@@ -2937,7 +2958,7 @@
       </c>
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>12</v>
       </c>
@@ -2956,7 +2977,7 @@
       </c>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>13</v>
       </c>
@@ -3030,29 +3051,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="7"/>
+    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
@@ -3068,40 +3089,40 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="80" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="K4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3115,7 +3136,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="57" t="s">
         <v>90</v>
@@ -3126,20 +3147,20 @@
       <c r="H5" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="84"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="6">
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 I2:J1048576">
     <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
@@ -3187,29 +3208,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="7"/>
+    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
@@ -3225,7 +3246,7 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>92</v>
       </c>
@@ -3237,37 +3258,37 @@
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="80" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="K4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3281,7 +3302,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="57" t="s">
         <v>90</v>
@@ -3292,20 +3313,20 @@
       <c r="H5" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="84"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="6">
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 I2:J2 I4:J1048576">
     <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
@@ -3352,29 +3373,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="7"/>
+    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
@@ -3390,40 +3411,40 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="80" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="K4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3437,7 +3458,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="57" t="s">
         <v>90</v>
@@ -3448,20 +3469,20 @@
       <c r="H5" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="84"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <mergeCells count="6">
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 I2:J1048576">
     <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
@@ -3508,29 +3529,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="7"/>
+    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
@@ -3546,40 +3567,40 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="80" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="K4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3593,7 +3614,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="57" t="s">
         <v>90</v>
@@ -3604,20 +3625,20 @@
       <c r="H5" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="84"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <mergeCells count="6">
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 I2:J1048576">
     <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
@@ -3664,29 +3685,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="7"/>
+    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>62</v>
       </c>
@@ -3702,40 +3723,40 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="80" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="K4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3749,7 +3770,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="57" t="s">
         <v>90</v>
@@ -3760,20 +3781,20 @@
       <c r="H5" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="84"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="6">
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 I2:J1048576">
     <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
@@ -3820,29 +3841,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="7"/>
+    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
@@ -3858,40 +3879,40 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="80" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="K4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3905,7 +3926,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="57" t="s">
         <v>90</v>
@@ -3916,20 +3937,20 @@
       <c r="H5" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="84"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <mergeCells count="6">
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 I2:J1048576">
     <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
@@ -3976,29 +3997,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="7"/>
+    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
@@ -4014,40 +4035,40 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="80" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="K4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -4061,7 +4082,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="57" t="s">
         <v>90</v>
@@ -4072,10 +4093,10 @@
       <c r="H5" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="84"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
Create a unique function to get objects in CBTC Territory for all objects instead of many multiple functions doing very similar things. Modify survey window behavior to not close, to be able to modify the inputs on error and at the end of the verification, if finally something is wrong.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDCB5A6-54D5-420C-988A-D45AEE3D5430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2053829A-24FC-45F4-B537-6DA781A22092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>v1_6</t>
+    <t>v1_7</t>
   </si>
 </sst>
 </file>
@@ -2778,7 +2778,7 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:7" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
         <v>4</v>
       </c>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:7" ht="52.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="76"/>
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>

</xml_diff>

<commit_message>
Set version to v2_0
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2053829A-24FC-45F4-B537-6DA781A22092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB829D0-7F2E-49A5-9402-BB98E764475F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,7 +438,7 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>v1_7</t>
+    <t>v2_0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Error in previous commit, it corresponds to the same commit.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB829D0-7F2E-49A5-9402-BB98E764475F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B1C0AF-2DD4-47C7-8595-6161EA87CB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>v2_0</t>
+    <t>v2_1</t>
   </si>
 </sst>
 </file>
@@ -2396,29 +2396,29 @@
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.28515625" style="49" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="49" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" style="49" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="49"/>
+    <col min="1" max="2" width="16.33203125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="49" customWidth="1"/>
+    <col min="6" max="7" width="16.33203125" style="49" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G6" s="50"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="60" t="s">
         <v>6</v>
       </c>
@@ -2427,63 +2427,63 @@
       <c r="E13" s="61"/>
       <c r="F13" s="62"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="63"/>
       <c r="C14" s="64"/>
       <c r="D14" s="64"/>
       <c r="E14" s="64"/>
       <c r="F14" s="65"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="63"/>
       <c r="C15" s="64"/>
       <c r="D15" s="64"/>
       <c r="E15" s="64"/>
       <c r="F15" s="65"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="63"/>
       <c r="C16" s="64"/>
       <c r="D16" s="64"/>
       <c r="E16" s="64"/>
       <c r="F16" s="65"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="63"/>
       <c r="C17" s="64"/>
       <c r="D17" s="64"/>
       <c r="E17" s="64"/>
       <c r="F17" s="65"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="63"/>
       <c r="C18" s="64"/>
       <c r="D18" s="64"/>
       <c r="E18" s="64"/>
       <c r="F18" s="65"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="63"/>
       <c r="C19" s="64"/>
       <c r="D19" s="64"/>
       <c r="E19" s="64"/>
       <c r="F19" s="65"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="66"/>
       <c r="C20" s="67"/>
       <c r="D20" s="67"/>
       <c r="E20" s="67"/>
       <c r="F20" s="68"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
       <c r="D21" s="53"/>
       <c r="E21" s="52"/>
       <c r="F21" s="52"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="53"/>
       <c r="C22" s="53"/>
       <c r="D22" s="53"/>
@@ -2491,7 +2491,7 @@
       <c r="F22" s="53"/>
       <c r="G22" s="53"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="53"/>
       <c r="C23" s="43" t="s">
         <v>0</v>
@@ -2505,7 +2505,7 @@
       <c r="F23" s="53"/>
       <c r="G23" s="53"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="53"/>
       <c r="C24" s="44"/>
       <c r="D24" s="44"/>
@@ -2513,7 +2513,7 @@
       <c r="F24" s="53"/>
       <c r="G24" s="53"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
       <c r="D25" s="53"/>
@@ -2521,7 +2521,7 @@
       <c r="F25" s="53"/>
       <c r="G25" s="53"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
       <c r="D26" s="53"/>
@@ -2529,21 +2529,21 @@
       <c r="F26" s="53"/>
       <c r="G26" s="53"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="45" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="46"/>
       <c r="E27" s="53"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="47" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="46"/>
       <c r="E28" s="53"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="47" t="s">
         <v>89</v>
       </c>
@@ -2552,7 +2552,7 @@
       </c>
       <c r="E29" s="53"/>
     </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="45" t="s">
         <v>5</v>
       </c>
@@ -2578,14 +2578,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="3"/>
-    <col min="2" max="2" width="121.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5703125" style="3"/>
+    <col min="1" max="1" width="11.5546875" style="3"/>
+    <col min="2" max="2" width="121.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>56</v>
       </c>
@@ -2673,19 +2673,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="42" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="42" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="42" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="41" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="42" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="42" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" style="42" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="41" customWidth="1"/>
     <col min="6" max="6" width="30" style="42" customWidth="1"/>
-    <col min="7" max="7" width="108.140625" style="42" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="21"/>
+    <col min="7" max="7" width="108.109375" style="42" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -2727,7 +2727,7 @@
       </c>
       <c r="G2" s="26"/>
     </row>
-    <row r="3" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="75">
         <v>2</v>
       </c>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:7" ht="77.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="76"/>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="G4" s="59"/>
     </row>
-    <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -2778,7 +2778,7 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="75">
         <v>4</v>
       </c>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="76"/>
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="G7" s="30"/>
     </row>
-    <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A10" s="75">
         <v>7</v>
       </c>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="G10" s="71"/>
     </row>
-    <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="79"/>
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
@@ -2880,7 +2880,7 @@
       <c r="F11" s="70"/>
       <c r="G11" s="72"/>
     </row>
-    <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22">
         <v>8</v>
       </c>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="G12" s="37"/>
     </row>
-    <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="22">
         <v>9</v>
       </c>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
         <v>10</v>
       </c>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="22">
         <v>11</v>
       </c>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="22">
         <v>12</v>
       </c>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="22">
         <v>13</v>
       </c>
@@ -3056,24 +3056,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
@@ -3089,14 +3089,14 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3213,24 +3213,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
@@ -3246,7 +3246,7 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>92</v>
       </c>
@@ -3258,11 +3258,11 @@
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3378,24 +3378,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
@@ -3411,14 +3411,14 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3534,24 +3534,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
@@ -3567,14 +3567,14 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3690,24 +3690,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>62</v>
       </c>
@@ -3723,14 +3723,14 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3846,24 +3846,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
@@ -3879,14 +3879,14 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -4002,24 +4002,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="33" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="15.88671875" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
@@ -4035,14 +4035,14 @@
       <c r="K1" s="8"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>47</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Block Def file is fully loaded, and checked with DC_SYS to find which limit name corresponds to which (track, kp) in DC_SYS. Use this block def limit name in order to find the survey name. Do the comparison with both TC and buffers. Create another survey result file with an extra column for joint sheet, in order to write the block def name. If the block def option is selected, it will use this template, else the old template without this extra column. Set different colors for buffers when used in the joint verif.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B1C0AF-2DD4-47C7-8595-6161EA87CB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF56F87-695F-4081-8B14-57892445EFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -3485,36 +3485,36 @@
     <mergeCell ref="E4:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 I2:J1048576">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="47" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="10" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1 J2:J1048576">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J1048576">
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1 L2:L1048576">
-    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Improve detection of not complete lines in pdf parsing. Split dc_par folder. Re-work Survey Window colors. Change log color to be more visible. Change behavior when asking Y/N to user, in order to wait for an actual Y or N, instead of just checking if it is a Y. Develop function to verify CBTC Protecting Switch Area. Develop function to get max slope in overshoot recovery areas.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D4671C5-EB19-44D7-8286-50389F0933C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAD569D0-0482-4F68-A452-22EAC862E01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -1840,23 +1840,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>746984</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>154753</xdr:rowOff>
+      <xdr:colOff>1513915</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>188819</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="Hitachi_Hitachi_STS_orizz_Project_and_External_Documents_Orizzontale">
+        <xdr:cNvPr id="3" name="Image 2" descr="Hitachi_Hitachi_STS_orizz_Project_and_External_Documents_Orizzontale">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2327E093-F453-4E8B-BD70-4C6A9B1DC1CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1879,8 +1879,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="320040" y="350520"/>
-          <a:ext cx="4522470" cy="375285"/>
+          <a:off x="1086971" y="605118"/>
+          <a:ext cx="4416238" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2183,7 +2183,7 @@
   </sheetPr>
   <dimension ref="A6:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Re-work of survey verification for floodgates using the same principle as platform extremities and block definition association. Create generic functions to work for both platform and floodgates.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAD569D0-0482-4F68-A452-22EAC862E01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF4A8A22-AE63-4F3D-98F4-273A4C3C3A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,25 +592,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FF9999FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFE699"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FFC6E0B4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9999FF"/>
+        <fgColor rgb="FFBDD7EE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1064,17 +1064,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1172,116 +1163,125 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1820,6 +1820,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBDD7EE"/>
+      <color rgb="FFC6E0B4"/>
+      <color rgb="FFFFE699"/>
+      <color rgb="FFBFBFBF"/>
       <color rgb="FF9999FF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFCC66FF"/>
@@ -1918,7 +1922,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1932,7 +1936,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -1944,7 +1948,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -2189,164 +2193,164 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.28515625" style="40" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="40" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" style="40" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="40"/>
+    <col min="1" max="2" width="16.28515625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="37" customWidth="1"/>
+    <col min="6" max="7" width="16.28515625" style="37" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="37"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="41"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="39"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="56"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="56"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="57"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="52"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
-      <c r="C23" s="34" t="s">
+      <c r="B23" s="41"/>
+      <c r="C23" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
     </row>
     <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="44"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
     </row>
     <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
     </row>
     <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="44"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="41"/>
     </row>
     <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="44"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="41"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="44"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="41"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="44"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2372,326 +2376,326 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="33" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="33" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="30" style="33" customWidth="1"/>
-    <col min="7" max="7" width="108.140625" style="33" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="12"/>
+    <col min="1" max="1" width="7.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" style="30" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="30" style="30" customWidth="1"/>
+    <col min="7" max="7" width="108.140625" style="30" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66">
+      <c r="A3" s="59">
         <v>2</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="77.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="14" t="s">
+      <c r="A4" s="60"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="49" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="23" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="21"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="66">
+      <c r="A6" s="59">
         <v>4</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="20" t="s">
+      <c r="E6" s="21"/>
+      <c r="F6" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="67"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="23" t="s">
+      <c r="A7" s="60"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="21"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="10">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="25" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="10">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="66">
+      <c r="A10" s="59">
         <v>7</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="62"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="28" t="s">
+      <c r="A11" s="63"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="63"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="56"/>
     </row>
     <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="10">
         <v>8</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="28"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="10">
         <v>9</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="30" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="21"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14" s="10">
         <v>10</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="30" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="21"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15" s="10">
         <v>11</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="30" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
+      <c r="A16" s="10">
         <v>12</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="25" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
+      <c r="A17" s="10">
         <v>13</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="25" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
@@ -2780,7 +2784,7 @@
       <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -2794,60 +2798,60 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="78" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -2937,7 +2941,7 @@
       <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -2960,60 +2964,60 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="78" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3102,7 +3106,7 @@
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -3116,60 +3120,60 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="78" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -3258,7 +3262,7 @@
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -3272,60 +3276,60 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="78" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -3414,7 +3418,7 @@
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -3428,60 +3432,60 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="78" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -3570,7 +3574,7 @@
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -3584,60 +3588,60 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="78" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -3726,7 +3730,7 @@
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -3740,60 +3744,60 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="78" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
Fix a bug when Block Def. file is not matching DC_SYS. Remove comment when an object appears twice in survey but with the same value. Reorder tracks in survey to take into account numbers inside the names: Track_10, 11, ..., 19 were ordered before Track_2.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF4A8A22-AE63-4F3D-98F4-273A4C3C3A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8105F531-4DBC-4745-B3D5-3B83EBDFD0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -1169,6 +1169,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1238,13 +1259,22 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1252,36 +1282,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1293,7 +1293,7 @@
     <cellStyle name="Normal 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 6 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="52">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1326,13 +1326,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1353,13 +1346,14 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
+        <i val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -1394,13 +1388,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1421,13 +1408,14 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
+        <i val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -1462,13 +1450,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1489,13 +1470,14 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
+        <i val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -1530,13 +1512,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1557,13 +1532,14 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
+        <i val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -1598,13 +1574,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1625,12 +1594,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="5"/>
       </font>
     </dxf>
@@ -1639,11 +1602,6 @@
         <b/>
         <i val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -1678,13 +1636,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1705,13 +1656,14 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
+        <i val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -1746,13 +1698,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1773,13 +1718,13 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -1920,7 +1865,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1960,7 +1905,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1995,6 +1940,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2030,9 +1992,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2174,7 +2153,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2187,98 +2166,98 @@
   </sheetPr>
   <dimension ref="A6:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.28515625" style="37" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="37" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" style="37" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="37"/>
+    <col min="1" max="2" width="16.33203125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="37" customWidth="1"/>
+    <col min="6" max="7" width="16.33203125" style="37" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="37"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="s">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
-    </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="49"/>
-    </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="49"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="52"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
@@ -2286,7 +2265,7 @@
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="41"/>
       <c r="C23" s="31" t="s">
         <v>0</v>
@@ -2300,7 +2279,7 @@
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="41"/>
       <c r="C24" s="32"/>
       <c r="D24" s="32"/>
@@ -2308,7 +2287,7 @@
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
@@ -2316,7 +2295,7 @@
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -2324,28 +2303,28 @@
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="33" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="41"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="35" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="41"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="33" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="41"/>
     </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="35" t="s">
         <v>85</v>
       </c>
@@ -2374,19 +2353,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="30" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="30" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" style="30" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="29" customWidth="1"/>
     <col min="6" max="6" width="30" style="30" customWidth="1"/>
-    <col min="7" max="7" width="108.140625" style="30" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="9"/>
+    <col min="7" max="7" width="108.109375" style="30" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -2409,7 +2388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -2428,14 +2407,14 @@
       </c>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59">
+    <row r="3" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="66">
         <v>2</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="68" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="15" t="s">
@@ -2447,10 +2426,10 @@
       </c>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="77.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
+    <row r="4" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="11" t="s">
         <v>79</v>
       </c>
@@ -2460,7 +2439,7 @@
       </c>
       <c r="G4" s="43"/>
     </row>
-    <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -2479,17 +2458,17 @@
       </c>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="59">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="66">
         <v>4</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="68" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="21"/>
@@ -2498,18 +2477,18 @@
       </c>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="60"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
+    <row r="7" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="67"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
       <c r="E7" s="12"/>
       <c r="F7" s="20" t="s">
         <v>49</v>
       </c>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -2528,7 +2507,7 @@
       </c>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>6</v>
       </c>
@@ -2549,39 +2528,39 @@
       </c>
       <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="59">
+    <row r="10" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="66">
         <v>7</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="68" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
+      <c r="G10" s="62"/>
+    </row>
+    <row r="11" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="70"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="56"/>
-    </row>
-    <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="65"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="63"/>
+    </row>
+    <row r="12" spans="1:7" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>8</v>
       </c>
@@ -2602,7 +2581,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>9</v>
       </c>
@@ -2621,7 +2600,7 @@
       </c>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>10</v>
       </c>
@@ -2640,7 +2619,7 @@
       </c>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>11</v>
       </c>
@@ -2659,7 +2638,7 @@
       </c>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>12</v>
       </c>
@@ -2678,7 +2657,7 @@
       </c>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>13</v>
       </c>
@@ -2715,13 +2694,13 @@
     <mergeCell ref="D6:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2742,6 +2721,7 @@
     <hyperlink ref="F4" location="Platform!A1" display="A: Sheet &quot;Platform&quot;" xr:uid="{484FCF78-BADC-448A-A37D-AFA47AC86165}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2757,24 +2737,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2790,68 +2770,68 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="70" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="74" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -2863,37 +2843,28 @@
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:I1 I2:J1048576">
-    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1 J2:J1048576">
-    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J1048576">
-    <cfRule type="cellIs" dxfId="53" priority="12" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 L2:L1048576">
-    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="11" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2914,24 +2885,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2947,7 +2918,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -2959,65 +2930,65 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="70" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="74" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -3029,37 +3000,28 @@
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:I1 I2:J2 I4:J1048576">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1 J2 J4:J1048576">
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J2 I4:J1048576">
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 L2 L4:L1048576">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3079,24 +3041,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -3112,68 +3074,68 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="70" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="74" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -3185,37 +3147,30 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:I1 I2:J1048576">
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1 J2:J1048576">
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J1048576">
-    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 L2:L1048576">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3235,24 +3190,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -3268,68 +3223,68 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="70" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="74" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -3341,37 +3296,28 @@
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:I1 I2:J1048576">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1 J2:J1048576">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J1048576">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 L2:L1048576">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3391,24 +3337,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -3424,68 +3370,68 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="70" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="74" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -3497,37 +3443,28 @@
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:I1 I2:J1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1 J2:J1048576">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J1048576">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 L2:L1048576">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3547,24 +3484,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -3580,68 +3517,68 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="70" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="74" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
@@ -3653,37 +3590,28 @@
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:I1 I2:J1048576">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1 J2:J1048576">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J1048576">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 L2:L1048576">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3703,24 +3631,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3736,68 +3664,68 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="70" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="74" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L5" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
@@ -3809,37 +3737,28 @@
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:I1 I2:J1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"Not Surveyed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1 J2:J1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J1048576">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
-      <formula>"Not Surveyed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 L2:L1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Improve CC checksum regeneration behavior, following the User Guide. Fix survey verif for: a problem in the template in the conditional formatting, and the behavior to get the tolerance variable name for plt ends/osps to work also when object is only in survey and not in dc_sys, and the variable dc_sys_sheet is None.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8105F531-4DBC-4745-B3D5-3B83EBDFD0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C290BA3-CA35-4878-9E20-37E573849DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -1293,7 +1293,7 @@
     <cellStyle name="Normal 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 6 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="62">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1760,6 +1760,93 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2170,29 +2257,29 @@
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.33203125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="37" customWidth="1"/>
-    <col min="6" max="7" width="16.33203125" style="37" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="37"/>
+    <col min="1" max="2" width="16.28515625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="37" customWidth="1"/>
+    <col min="6" max="7" width="16.28515625" style="37" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="37"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="39"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="51" t="s">
         <v>6</v>
       </c>
@@ -2201,63 +2288,63 @@
       <c r="E13" s="52"/>
       <c r="F13" s="53"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="54"/>
       <c r="C14" s="55"/>
       <c r="D14" s="55"/>
       <c r="E14" s="55"/>
       <c r="F14" s="56"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="54"/>
       <c r="C15" s="55"/>
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="F15" s="56"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="54"/>
       <c r="C16" s="55"/>
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
       <c r="F16" s="56"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="54"/>
       <c r="C17" s="55"/>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="56"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="54"/>
       <c r="C18" s="55"/>
       <c r="D18" s="55"/>
       <c r="E18" s="55"/>
       <c r="F18" s="56"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="54"/>
       <c r="C19" s="55"/>
       <c r="D19" s="55"/>
       <c r="E19" s="55"/>
       <c r="F19" s="56"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="57"/>
       <c r="C20" s="58"/>
       <c r="D20" s="58"/>
       <c r="E20" s="58"/>
       <c r="F20" s="59"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
@@ -2265,7 +2352,7 @@
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="41"/>
       <c r="C23" s="31" t="s">
         <v>0</v>
@@ -2279,7 +2366,7 @@
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="41"/>
       <c r="C24" s="32"/>
       <c r="D24" s="32"/>
@@ -2287,7 +2374,7 @@
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
@@ -2295,7 +2382,7 @@
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -2303,28 +2390,28 @@
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="33" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="41"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="35" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="41"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="33" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="41"/>
     </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="35" t="s">
         <v>85</v>
       </c>
@@ -2353,19 +2440,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" style="30" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="49.88671875" style="30" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" style="30" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="29" customWidth="1"/>
     <col min="6" max="6" width="30" style="30" customWidth="1"/>
-    <col min="7" max="7" width="108.109375" style="30" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="9"/>
+    <col min="7" max="7" width="108.140625" style="30" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -2388,7 +2475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -2407,7 +2494,7 @@
       </c>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66">
         <v>2</v>
       </c>
@@ -2426,7 +2513,7 @@
       </c>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="77.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="67"/>
       <c r="B4" s="69"/>
       <c r="C4" s="69"/>
@@ -2439,7 +2526,7 @@
       </c>
       <c r="G4" s="43"/>
     </row>
-    <row r="5" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -2458,7 +2545,7 @@
       </c>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="66">
         <v>4</v>
       </c>
@@ -2477,7 +2564,7 @@
       </c>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="67"/>
       <c r="B7" s="69"/>
       <c r="C7" s="69"/>
@@ -2488,7 +2575,7 @@
       </c>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -2507,7 +2594,7 @@
       </c>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>6</v>
       </c>
@@ -2528,7 +2615,7 @@
       </c>
       <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A10" s="66">
         <v>7</v>
       </c>
@@ -2549,7 +2636,7 @@
       </c>
       <c r="G10" s="62"/>
     </row>
-    <row r="11" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="70"/>
       <c r="B11" s="69"/>
       <c r="C11" s="69"/>
@@ -2560,7 +2647,7 @@
       <c r="F11" s="61"/>
       <c r="G11" s="63"/>
     </row>
-    <row r="12" spans="1:7" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>8</v>
       </c>
@@ -2581,7 +2668,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>9</v>
       </c>
@@ -2600,7 +2687,7 @@
       </c>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>10</v>
       </c>
@@ -2619,7 +2706,7 @@
       </c>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>11</v>
       </c>
@@ -2638,7 +2725,7 @@
       </c>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>12</v>
       </c>
@@ -2657,7 +2744,7 @@
       </c>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>13</v>
       </c>
@@ -2737,24 +2824,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2770,14 +2857,14 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
@@ -2803,7 +2890,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
@@ -2885,24 +2972,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2918,7 +3005,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -2930,11 +3017,11 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
@@ -2960,7 +3047,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
@@ -3041,24 +3128,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -3074,14 +3161,14 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
@@ -3107,7 +3194,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
@@ -3147,12 +3234,10 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
   </mergeCells>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="I1:J1048576">
     <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Not Surveyed"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:J1048576">
     <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Not in DC_SYS"</formula>
     </cfRule>
@@ -3190,24 +3275,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -3223,14 +3308,14 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
@@ -3256,7 +3341,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
@@ -3337,24 +3422,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -3370,14 +3455,14 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
@@ -3403,7 +3488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
@@ -3484,24 +3569,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -3517,14 +3602,14 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
@@ -3550,7 +3635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>40</v>
       </c>
@@ -3631,24 +3716,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3664,14 +3749,14 @@
       <c r="K1" s="3"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
@@ -3697,7 +3782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Survey_Verification v2.5.2: Add list of survey files in the Header sheet. Improve correspondence spaces to underscores and add underscore between letters and numbers, e.g. TK02 -> TK_02 for both survey track names and survey object names, after testing on Lima. Systemize the use of r"" raw strings for regular expressions, when doing a re.sub.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_survey_verification.xlsx
+++ b/prj/src/templates/template_survey_verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E823FCA3-3E80-4D3C-B7A4-B1B5AE7A76BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62A1795-236A-4E60-A2FE-E55DDD76268C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3DDC2E89-A160-455D-8CEC-48C24A43E069}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Correspondence with Site Survey</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>Localization Tags positioning</t>
+  </si>
+  <si>
+    <t>Survey:</t>
   </si>
 </sst>
 </file>
@@ -771,6 +774,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -798,6 +817,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -824,25 +846,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -910,7 +913,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>255518</xdr:colOff>
+      <xdr:colOff>36443</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>131174</xdr:rowOff>
     </xdr:to>
@@ -1268,7 +1271,7 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="B13:F30"/>
+  <dimension ref="B13:F31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:F20"/>
@@ -1276,68 +1279,68 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="40"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
@@ -1368,16 +1371,22 @@
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D31" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1402,14 +1411,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="48" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" style="48" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="48" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="48" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="50" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="48" customWidth="1"/>
-    <col min="7" max="7" width="100.7109375" style="48" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="48"/>
+    <col min="1" max="1" width="7.7109375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="29" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="29" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="31" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="100.7109375" style="29" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1449,39 +1458,39 @@
         <v>17</v>
       </c>
       <c r="E2" s="13"/>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="30" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
+      <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="48" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="16"/>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="26" t="s">
         <v>62</v>
       </c>
       <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="27" t="s">
         <v>61</v>
       </c>
       <c r="G4" s="19"/>
@@ -1500,39 +1509,39 @@
         <v>24</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="30" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="46">
         <v>4</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="48" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="24"/>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="26" t="s">
         <v>63</v>
       </c>
       <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="53.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="19" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="25"/>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="27" t="s">
         <v>64</v>
       </c>
       <c r="G7" s="19"/>
@@ -1551,7 +1560,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="28" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="17"/>
@@ -1578,36 +1587,36 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39">
+      <c r="A10" s="46">
         <v>7</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="48" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="35"/>
+      <c r="G10" s="42"/>
     </row>
     <row r="11" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="36"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="43"/>
     </row>
     <row r="12" spans="1:7" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
@@ -1644,7 +1653,7 @@
         <v>44</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="30" t="s">
         <v>66</v>
       </c>
       <c r="G13" s="17"/>
@@ -1663,7 +1672,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="13"/>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G14" s="17"/>
@@ -1682,7 +1691,7 @@
         <v>48</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="30" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="17"/>

</xml_diff>